<commit_message>
wip: fixes on header parse, tweaks
</commit_message>
<xml_diff>
--- a/Data/input_dir_sample/Template.xlsx
+++ b/Data/input_dir_sample/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6750" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="KYTH031404040620.EW1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:U12021"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +493,6 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="e">
-        <f>B4+4</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="E4" s="2"/>
       <c r="I4" s="2"/>
       <c r="M4" s="2"/>
@@ -542,10 +538,6 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="e">
-        <f t="shared" ref="C5:C19" si="0">B9+4</f>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -578,10 +570,6 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -590,10 +578,6 @@
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -618,10 +602,6 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -634,10 +614,6 @@
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>20</v>
-      </c>
-      <c r="C19" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>